<commit_message>
Points List Print Area Set
</commit_message>
<xml_diff>
--- a/SARAJI_MINE_Points_List_RevA.xlsx
+++ b/SARAJI_MINE_Points_List_RevA.xlsx
@@ -117,8 +117,8 @@
     <definedName name="ModelNumber" localSheetId="2">'AC2'!$D$5</definedName>
     <definedName name="Options" localSheetId="1">'AC1'!$AA:$AK</definedName>
     <definedName name="Options" localSheetId="2">'AC2'!$AA:$AK</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'AC1'!$A$1:$N$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'AC2'!$A$1:$N$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'AC1'!$A$1:$M$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'AC2'!$A$1:$M$37</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'AC1'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'AC2'!$1:$1</definedName>
     <definedName name="ProjectName">Project!$B$1</definedName>
@@ -2570,7 +2570,7 @@
   <dimension ref="B1:AY43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection sqref="A1:M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4537,7 +4537,7 @@
   <dimension ref="B1:AY43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B37" sqref="A1:M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Requesting data from client
</commit_message>
<xml_diff>
--- a/SARAJI_MINE_Points_List_RevA.xlsx
+++ b/SARAJI_MINE_Points_List_RevA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="853" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="853" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="4" r:id="rId1"/>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="349">
   <si>
     <t>Project Name:</t>
   </si>
@@ -1198,6 +1198,9 @@
   </si>
   <si>
     <t>CO Sensor AC2</t>
+  </si>
+  <si>
+    <t>Afterhours Push Button</t>
   </si>
 </sst>
 </file>
@@ -1917,43 +1920,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1965,42 +1932,73 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2013,21 +2011,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2543,7 +2546,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="84" t="s">
         <v>324</v>
       </c>
     </row>
@@ -2569,8 +2572,8 @@
   </sheetPr>
   <dimension ref="B1:AY43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,261 +2624,261 @@
       <c r="K2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="101" t="str">
+      <c r="L2" s="94" t="str">
         <f>IF(ProjectNumber="","",ProjectNumber)</f>
         <v>---</v>
       </c>
-      <c r="M2" s="101"/>
+      <c r="M2" s="94"/>
     </row>
     <row r="3" spans="2:49" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.35">
       <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="96"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
       <c r="K3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="102" t="s">
+      <c r="L3" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="102"/>
+      <c r="M3" s="98"/>
     </row>
     <row r="4" spans="2:49" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.35">
       <c r="C4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="97"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="99"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="87"/>
       <c r="K4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="121" t="s">
+      <c r="L4" s="88" t="s">
         <v>325</v>
       </c>
-      <c r="M4" s="112"/>
+      <c r="M4" s="89"/>
     </row>
     <row r="5" spans="2:49" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.35">
       <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="100" t="s">
+      <c r="D5" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
     </row>
     <row r="6" spans="2:49" s="9" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:49" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84" t="s">
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="84" t="s">
+      <c r="J7" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="84" t="s">
+      <c r="K7" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="84" t="s">
+      <c r="L7" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="87" t="s">
+      <c r="M7" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="109" t="s">
+      <c r="P7" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="84"/>
-      <c r="S7" s="84"/>
-      <c r="T7" s="84"/>
-      <c r="U7" s="84"/>
-      <c r="V7" s="84"/>
-      <c r="W7" s="84"/>
-      <c r="X7" s="87"/>
-      <c r="AA7" s="109" t="s">
+      <c r="Q7" s="103"/>
+      <c r="R7" s="103"/>
+      <c r="S7" s="103"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="103"/>
+      <c r="V7" s="103"/>
+      <c r="W7" s="103"/>
+      <c r="X7" s="106"/>
+      <c r="AA7" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="AB7" s="84"/>
-      <c r="AC7" s="84"/>
-      <c r="AD7" s="84"/>
-      <c r="AE7" s="84" t="s">
+      <c r="AB7" s="103"/>
+      <c r="AC7" s="103"/>
+      <c r="AD7" s="103"/>
+      <c r="AE7" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="AF7" s="84" t="s">
+      <c r="AF7" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="AG7" s="84" t="s">
+      <c r="AG7" s="103" t="s">
         <v>42</v>
       </c>
       <c r="AH7" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="AI7" s="84" t="s">
+      <c r="AI7" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="AJ7" s="84"/>
+      <c r="AJ7" s="103"/>
       <c r="AK7" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="AL7" s="117" t="s">
+      <c r="AL7" s="108" t="s">
         <v>290</v>
       </c>
-      <c r="AM7" s="109" t="s">
+      <c r="AM7" s="100" t="s">
         <v>291</v>
       </c>
-      <c r="AN7" s="84"/>
-      <c r="AO7" s="84"/>
-      <c r="AP7" s="84"/>
-      <c r="AQ7" s="119"/>
+      <c r="AN7" s="103"/>
+      <c r="AO7" s="103"/>
+      <c r="AP7" s="103"/>
+      <c r="AQ7" s="110"/>
       <c r="AR7" s="46" t="s">
         <v>297</v>
       </c>
-      <c r="AS7" s="109" t="s">
+      <c r="AS7" s="100" t="s">
         <v>299</v>
       </c>
-      <c r="AT7" s="84"/>
-      <c r="AU7" s="84"/>
-      <c r="AV7" s="84"/>
-      <c r="AW7" s="87"/>
+      <c r="AT7" s="103"/>
+      <c r="AU7" s="103"/>
+      <c r="AV7" s="103"/>
+      <c r="AW7" s="106"/>
     </row>
     <row r="8" spans="2:49" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="110"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85" t="s">
+      <c r="B8" s="101"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="88"/>
-      <c r="P8" s="110" t="s">
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="107"/>
+      <c r="P8" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="85"/>
-      <c r="R8" s="85"/>
-      <c r="S8" s="85" t="s">
+      <c r="Q8" s="104"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="T8" s="85"/>
-      <c r="U8" s="85"/>
-      <c r="V8" s="85" t="s">
+      <c r="T8" s="104"/>
+      <c r="U8" s="104"/>
+      <c r="V8" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="W8" s="85"/>
-      <c r="X8" s="88"/>
-      <c r="AA8" s="110" t="s">
+      <c r="W8" s="104"/>
+      <c r="X8" s="107"/>
+      <c r="AA8" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="AB8" s="85" t="s">
+      <c r="AB8" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="AC8" s="85" t="s">
+      <c r="AC8" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="AD8" s="85" t="s">
+      <c r="AD8" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="AE8" s="85"/>
-      <c r="AF8" s="85"/>
-      <c r="AG8" s="85"/>
-      <c r="AH8" s="85" t="s">
+      <c r="AE8" s="104"/>
+      <c r="AF8" s="104"/>
+      <c r="AG8" s="104"/>
+      <c r="AH8" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="AI8" s="85" t="s">
+      <c r="AI8" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="AJ8" s="85" t="s">
+      <c r="AJ8" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="AK8" s="113" t="s">
+      <c r="AK8" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="AL8" s="118"/>
-      <c r="AM8" s="110" t="s">
+      <c r="AL8" s="109"/>
+      <c r="AM8" s="101" t="s">
         <v>292</v>
       </c>
-      <c r="AN8" s="85" t="s">
+      <c r="AN8" s="104" t="s">
         <v>293</v>
       </c>
-      <c r="AO8" s="85" t="s">
+      <c r="AO8" s="104" t="s">
         <v>294</v>
       </c>
-      <c r="AP8" s="85" t="s">
+      <c r="AP8" s="104" t="s">
         <v>295</v>
       </c>
-      <c r="AQ8" s="113" t="s">
+      <c r="AQ8" s="111" t="s">
         <v>296</v>
       </c>
-      <c r="AR8" s="115" t="s">
+      <c r="AR8" s="113" t="s">
         <v>298</v>
       </c>
-      <c r="AS8" s="110" t="s">
+      <c r="AS8" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="AT8" s="85" t="s">
+      <c r="AT8" s="104" t="s">
         <v>301</v>
       </c>
-      <c r="AU8" s="85" t="s">
+      <c r="AU8" s="104" t="s">
         <v>302</v>
       </c>
-      <c r="AV8" s="85" t="s">
+      <c r="AV8" s="104" t="s">
         <v>303</v>
       </c>
-      <c r="AW8" s="88" t="s">
+      <c r="AW8" s="107" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="9" spans="2:49" s="5" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="111"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="89"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="115"/>
       <c r="P9" s="67" t="s">
         <v>26</v>
       </c>
@@ -2903,29 +2906,29 @@
       <c r="X9" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="AA9" s="111"/>
-      <c r="AB9" s="86"/>
-      <c r="AC9" s="86"/>
-      <c r="AD9" s="86"/>
-      <c r="AE9" s="86"/>
-      <c r="AF9" s="86"/>
-      <c r="AG9" s="86"/>
-      <c r="AH9" s="86"/>
-      <c r="AI9" s="86"/>
-      <c r="AJ9" s="86"/>
-      <c r="AK9" s="114"/>
-      <c r="AL9" s="118"/>
-      <c r="AM9" s="111"/>
-      <c r="AN9" s="86"/>
-      <c r="AO9" s="86"/>
-      <c r="AP9" s="86"/>
-      <c r="AQ9" s="114"/>
-      <c r="AR9" s="116"/>
-      <c r="AS9" s="111"/>
-      <c r="AT9" s="86"/>
-      <c r="AU9" s="86"/>
-      <c r="AV9" s="86"/>
-      <c r="AW9" s="89"/>
+      <c r="AA9" s="102"/>
+      <c r="AB9" s="105"/>
+      <c r="AC9" s="105"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="105"/>
+      <c r="AG9" s="105"/>
+      <c r="AH9" s="105"/>
+      <c r="AI9" s="105"/>
+      <c r="AJ9" s="105"/>
+      <c r="AK9" s="112"/>
+      <c r="AL9" s="109"/>
+      <c r="AM9" s="102"/>
+      <c r="AN9" s="105"/>
+      <c r="AO9" s="105"/>
+      <c r="AP9" s="105"/>
+      <c r="AQ9" s="112"/>
+      <c r="AR9" s="114"/>
+      <c r="AS9" s="102"/>
+      <c r="AT9" s="105"/>
+      <c r="AU9" s="105"/>
+      <c r="AV9" s="105"/>
+      <c r="AW9" s="115"/>
     </row>
     <row r="10" spans="2:49" s="5" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
@@ -3342,7 +3345,9 @@
         <v>307</v>
       </c>
       <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
+      <c r="D18" s="43" t="s">
+        <v>348</v>
+      </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -4155,46 +4160,46 @@
       </c>
     </row>
     <row r="35" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B35" s="103"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="104"/>
-      <c r="I35" s="104"/>
-      <c r="J35" s="104"/>
-      <c r="K35" s="104"/>
-      <c r="L35" s="104"/>
-      <c r="M35" s="105"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="117"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="117"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="117"/>
+      <c r="L35" s="117"/>
+      <c r="M35" s="118"/>
     </row>
     <row r="36" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B36" s="106"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="107"/>
-      <c r="F36" s="107"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="107"/>
-      <c r="I36" s="107"/>
-      <c r="J36" s="107"/>
-      <c r="K36" s="107"/>
-      <c r="L36" s="107"/>
-      <c r="M36" s="108"/>
+      <c r="B36" s="119"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="120"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="120"/>
+      <c r="I36" s="120"/>
+      <c r="J36" s="120"/>
+      <c r="K36" s="120"/>
+      <c r="L36" s="120"/>
+      <c r="M36" s="121"/>
     </row>
     <row r="37" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B37" s="106"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="107"/>
-      <c r="E37" s="107"/>
-      <c r="F37" s="107"/>
-      <c r="G37" s="107"/>
-      <c r="H37" s="107"/>
-      <c r="I37" s="107"/>
-      <c r="J37" s="107"/>
-      <c r="K37" s="107"/>
-      <c r="L37" s="107"/>
-      <c r="M37" s="108"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="120"/>
+      <c r="F37" s="120"/>
+      <c r="G37" s="120"/>
+      <c r="H37" s="120"/>
+      <c r="I37" s="120"/>
+      <c r="J37" s="120"/>
+      <c r="K37" s="120"/>
+      <c r="L37" s="120"/>
+      <c r="M37" s="121"/>
     </row>
     <row r="38" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
@@ -4408,23 +4413,28 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="B36:M36"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="AA7:AD7"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="AU8:AU9"/>
+    <mergeCell ref="AV8:AV9"/>
+    <mergeCell ref="AW8:AW9"/>
+    <mergeCell ref="AS8:AS9"/>
+    <mergeCell ref="AT8:AT9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="AO8:AO9"/>
+    <mergeCell ref="AP8:AP9"/>
+    <mergeCell ref="AQ8:AQ9"/>
+    <mergeCell ref="AR8:AR9"/>
+    <mergeCell ref="AJ8:AJ9"/>
+    <mergeCell ref="AK8:AK9"/>
+    <mergeCell ref="AM8:AM9"/>
+    <mergeCell ref="AN8:AN9"/>
     <mergeCell ref="AS7:AW7"/>
     <mergeCell ref="P8:R8"/>
     <mergeCell ref="S8:U8"/>
@@ -4441,28 +4451,23 @@
     <mergeCell ref="AI7:AJ7"/>
     <mergeCell ref="AL7:AL9"/>
     <mergeCell ref="AM7:AQ7"/>
-    <mergeCell ref="AO8:AO9"/>
-    <mergeCell ref="AP8:AP9"/>
-    <mergeCell ref="AQ8:AQ9"/>
-    <mergeCell ref="AR8:AR9"/>
-    <mergeCell ref="AJ8:AJ9"/>
-    <mergeCell ref="AK8:AK9"/>
-    <mergeCell ref="AM8:AM9"/>
-    <mergeCell ref="AN8:AN9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="P7:X7"/>
-    <mergeCell ref="AA7:AD7"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="AU8:AU9"/>
-    <mergeCell ref="AV8:AV9"/>
-    <mergeCell ref="AW8:AW9"/>
-    <mergeCell ref="AS8:AS9"/>
-    <mergeCell ref="AT8:AT9"/>
-    <mergeCell ref="B36:M36"/>
-    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <dataValidations count="17">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Signal Type Input Error" error="The User entered an invalid value for the Signal Type" promptTitle="Select Signal Type" prompt="Select a Signal Type from the drop down list" sqref="I10:I21">
@@ -4536,8 +4541,8 @@
   </sheetPr>
   <dimension ref="B1:AY43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="A1:M37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4588,261 +4593,261 @@
       <c r="K2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="101" t="str">
+      <c r="L2" s="94" t="str">
         <f>IF(ProjectNumber="","",ProjectNumber)</f>
         <v>---</v>
       </c>
-      <c r="M2" s="101"/>
+      <c r="M2" s="94"/>
     </row>
     <row r="3" spans="2:49" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="96"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
       <c r="K3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="102" t="s">
+      <c r="L3" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="102"/>
+      <c r="M3" s="98"/>
     </row>
     <row r="4" spans="2:49" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="97"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="99"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="87"/>
       <c r="K4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="121" t="s">
+      <c r="L4" s="88" t="s">
         <v>325</v>
       </c>
-      <c r="M4" s="112"/>
+      <c r="M4" s="89"/>
     </row>
     <row r="5" spans="2:49" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="100" t="s">
+      <c r="D5" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
     </row>
     <row r="6" spans="2:49" s="9" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:49" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84" t="s">
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="84" t="s">
+      <c r="J7" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="84" t="s">
+      <c r="K7" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="84" t="s">
+      <c r="L7" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="87" t="s">
+      <c r="M7" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="109" t="s">
+      <c r="P7" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="84"/>
-      <c r="S7" s="84"/>
-      <c r="T7" s="84"/>
-      <c r="U7" s="84"/>
-      <c r="V7" s="84"/>
-      <c r="W7" s="84"/>
-      <c r="X7" s="87"/>
-      <c r="AA7" s="109" t="s">
+      <c r="Q7" s="103"/>
+      <c r="R7" s="103"/>
+      <c r="S7" s="103"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="103"/>
+      <c r="V7" s="103"/>
+      <c r="W7" s="103"/>
+      <c r="X7" s="106"/>
+      <c r="AA7" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="AB7" s="84"/>
-      <c r="AC7" s="84"/>
-      <c r="AD7" s="84"/>
-      <c r="AE7" s="84" t="s">
+      <c r="AB7" s="103"/>
+      <c r="AC7" s="103"/>
+      <c r="AD7" s="103"/>
+      <c r="AE7" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="AF7" s="84" t="s">
+      <c r="AF7" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="AG7" s="84" t="s">
+      <c r="AG7" s="103" t="s">
         <v>42</v>
       </c>
       <c r="AH7" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="AI7" s="84" t="s">
+      <c r="AI7" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="AJ7" s="84"/>
+      <c r="AJ7" s="103"/>
       <c r="AK7" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="AL7" s="117" t="s">
+      <c r="AL7" s="108" t="s">
         <v>290</v>
       </c>
-      <c r="AM7" s="109" t="s">
+      <c r="AM7" s="100" t="s">
         <v>291</v>
       </c>
-      <c r="AN7" s="84"/>
-      <c r="AO7" s="84"/>
-      <c r="AP7" s="84"/>
-      <c r="AQ7" s="119"/>
+      <c r="AN7" s="103"/>
+      <c r="AO7" s="103"/>
+      <c r="AP7" s="103"/>
+      <c r="AQ7" s="110"/>
       <c r="AR7" s="46" t="s">
         <v>297</v>
       </c>
-      <c r="AS7" s="109" t="s">
+      <c r="AS7" s="100" t="s">
         <v>299</v>
       </c>
-      <c r="AT7" s="84"/>
-      <c r="AU7" s="84"/>
-      <c r="AV7" s="84"/>
-      <c r="AW7" s="87"/>
+      <c r="AT7" s="103"/>
+      <c r="AU7" s="103"/>
+      <c r="AV7" s="103"/>
+      <c r="AW7" s="106"/>
     </row>
     <row r="8" spans="2:49" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="110"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85" t="s">
+      <c r="B8" s="101"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="88"/>
-      <c r="P8" s="110" t="s">
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="107"/>
+      <c r="P8" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="85"/>
-      <c r="R8" s="85"/>
-      <c r="S8" s="85" t="s">
+      <c r="Q8" s="104"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="T8" s="85"/>
-      <c r="U8" s="85"/>
-      <c r="V8" s="85" t="s">
+      <c r="T8" s="104"/>
+      <c r="U8" s="104"/>
+      <c r="V8" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="W8" s="85"/>
-      <c r="X8" s="88"/>
-      <c r="AA8" s="110" t="s">
+      <c r="W8" s="104"/>
+      <c r="X8" s="107"/>
+      <c r="AA8" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="AB8" s="85" t="s">
+      <c r="AB8" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="AC8" s="85" t="s">
+      <c r="AC8" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="AD8" s="85" t="s">
+      <c r="AD8" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="AE8" s="85"/>
-      <c r="AF8" s="85"/>
-      <c r="AG8" s="85"/>
-      <c r="AH8" s="85" t="s">
+      <c r="AE8" s="104"/>
+      <c r="AF8" s="104"/>
+      <c r="AG8" s="104"/>
+      <c r="AH8" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="AI8" s="85" t="s">
+      <c r="AI8" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="AJ8" s="85" t="s">
+      <c r="AJ8" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="AK8" s="113" t="s">
+      <c r="AK8" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="AL8" s="118"/>
-      <c r="AM8" s="110" t="s">
+      <c r="AL8" s="109"/>
+      <c r="AM8" s="101" t="s">
         <v>292</v>
       </c>
-      <c r="AN8" s="85" t="s">
+      <c r="AN8" s="104" t="s">
         <v>293</v>
       </c>
-      <c r="AO8" s="85" t="s">
+      <c r="AO8" s="104" t="s">
         <v>294</v>
       </c>
-      <c r="AP8" s="85" t="s">
+      <c r="AP8" s="104" t="s">
         <v>295</v>
       </c>
-      <c r="AQ8" s="113" t="s">
+      <c r="AQ8" s="111" t="s">
         <v>296</v>
       </c>
-      <c r="AR8" s="115" t="s">
+      <c r="AR8" s="113" t="s">
         <v>298</v>
       </c>
-      <c r="AS8" s="110" t="s">
+      <c r="AS8" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="AT8" s="85" t="s">
+      <c r="AT8" s="104" t="s">
         <v>301</v>
       </c>
-      <c r="AU8" s="85" t="s">
+      <c r="AU8" s="104" t="s">
         <v>302</v>
       </c>
-      <c r="AV8" s="85" t="s">
+      <c r="AV8" s="104" t="s">
         <v>303</v>
       </c>
-      <c r="AW8" s="88" t="s">
+      <c r="AW8" s="107" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="9" spans="2:49" s="5" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="111"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="89"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="115"/>
       <c r="P9" s="81" t="s">
         <v>26</v>
       </c>
@@ -4870,29 +4875,29 @@
       <c r="X9" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="AA9" s="111"/>
-      <c r="AB9" s="86"/>
-      <c r="AC9" s="86"/>
-      <c r="AD9" s="86"/>
-      <c r="AE9" s="86"/>
-      <c r="AF9" s="86"/>
-      <c r="AG9" s="86"/>
-      <c r="AH9" s="86"/>
-      <c r="AI9" s="86"/>
-      <c r="AJ9" s="86"/>
-      <c r="AK9" s="114"/>
-      <c r="AL9" s="118"/>
-      <c r="AM9" s="111"/>
-      <c r="AN9" s="86"/>
-      <c r="AO9" s="86"/>
-      <c r="AP9" s="86"/>
-      <c r="AQ9" s="114"/>
-      <c r="AR9" s="116"/>
-      <c r="AS9" s="111"/>
-      <c r="AT9" s="86"/>
-      <c r="AU9" s="86"/>
-      <c r="AV9" s="86"/>
-      <c r="AW9" s="89"/>
+      <c r="AA9" s="102"/>
+      <c r="AB9" s="105"/>
+      <c r="AC9" s="105"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="105"/>
+      <c r="AG9" s="105"/>
+      <c r="AH9" s="105"/>
+      <c r="AI9" s="105"/>
+      <c r="AJ9" s="105"/>
+      <c r="AK9" s="112"/>
+      <c r="AL9" s="109"/>
+      <c r="AM9" s="102"/>
+      <c r="AN9" s="105"/>
+      <c r="AO9" s="105"/>
+      <c r="AP9" s="105"/>
+      <c r="AQ9" s="112"/>
+      <c r="AR9" s="114"/>
+      <c r="AS9" s="102"/>
+      <c r="AT9" s="105"/>
+      <c r="AU9" s="105"/>
+      <c r="AV9" s="105"/>
+      <c r="AW9" s="115"/>
     </row>
     <row r="10" spans="2:49" s="5" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
@@ -5109,6 +5114,9 @@
         <v>54</v>
       </c>
       <c r="C14" s="43"/>
+      <c r="D14" s="5" t="s">
+        <v>348</v>
+      </c>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
@@ -6111,46 +6119,46 @@
       </c>
     </row>
     <row r="35" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B35" s="103"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="104"/>
-      <c r="I35" s="104"/>
-      <c r="J35" s="104"/>
-      <c r="K35" s="104"/>
-      <c r="L35" s="104"/>
-      <c r="M35" s="105"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="117"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="117"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="117"/>
+      <c r="L35" s="117"/>
+      <c r="M35" s="118"/>
     </row>
     <row r="36" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B36" s="106"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="107"/>
-      <c r="F36" s="107"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="107"/>
-      <c r="I36" s="107"/>
-      <c r="J36" s="107"/>
-      <c r="K36" s="107"/>
-      <c r="L36" s="107"/>
-      <c r="M36" s="108"/>
+      <c r="B36" s="119"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="120"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="120"/>
+      <c r="I36" s="120"/>
+      <c r="J36" s="120"/>
+      <c r="K36" s="120"/>
+      <c r="L36" s="120"/>
+      <c r="M36" s="121"/>
     </row>
     <row r="37" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B37" s="106"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="107"/>
-      <c r="E37" s="107"/>
-      <c r="F37" s="107"/>
-      <c r="G37" s="107"/>
-      <c r="H37" s="107"/>
-      <c r="I37" s="107"/>
-      <c r="J37" s="107"/>
-      <c r="K37" s="107"/>
-      <c r="L37" s="107"/>
-      <c r="M37" s="108"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="120"/>
+      <c r="F37" s="120"/>
+      <c r="G37" s="120"/>
+      <c r="H37" s="120"/>
+      <c r="I37" s="120"/>
+      <c r="J37" s="120"/>
+      <c r="K37" s="120"/>
+      <c r="L37" s="120"/>
+      <c r="M37" s="121"/>
     </row>
     <row r="38" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:51" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
@@ -6364,20 +6372,19 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B36:M36"/>
-    <mergeCell ref="B37:M37"/>
-    <mergeCell ref="AS8:AS9"/>
-    <mergeCell ref="AT8:AT9"/>
-    <mergeCell ref="AU8:AU9"/>
-    <mergeCell ref="AV8:AV9"/>
-    <mergeCell ref="AW8:AW9"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="AM8:AM9"/>
-    <mergeCell ref="AN8:AN9"/>
-    <mergeCell ref="AO8:AO9"/>
-    <mergeCell ref="AP8:AP9"/>
-    <mergeCell ref="AQ8:AQ9"/>
-    <mergeCell ref="AR8:AR9"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I7:I9"/>
     <mergeCell ref="AS7:AW7"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
@@ -6394,6 +6401,15 @@
     <mergeCell ref="AI7:AJ7"/>
     <mergeCell ref="AL7:AL9"/>
     <mergeCell ref="AM7:AQ7"/>
+    <mergeCell ref="AV8:AV9"/>
+    <mergeCell ref="AW8:AW9"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="AM8:AM9"/>
+    <mergeCell ref="AN8:AN9"/>
+    <mergeCell ref="AO8:AO9"/>
+    <mergeCell ref="AP8:AP9"/>
+    <mergeCell ref="AQ8:AQ9"/>
+    <mergeCell ref="AR8:AR9"/>
     <mergeCell ref="AH8:AH9"/>
     <mergeCell ref="AI8:AI9"/>
     <mergeCell ref="AJ8:AJ9"/>
@@ -6401,26 +6417,18 @@
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="L7:L9"/>
+    <mergeCell ref="B36:M36"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="AS8:AS9"/>
+    <mergeCell ref="AT8:AT9"/>
+    <mergeCell ref="AU8:AU9"/>
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="P7:X7"/>
     <mergeCell ref="AA7:AD7"/>
     <mergeCell ref="AC8:AC9"/>
     <mergeCell ref="AD8:AD9"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="L4:M4"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="17">
+  <dataValidations count="17">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Signal Type Input Error" error="The User entered an invalid value for the Signal Type" promptTitle="Select Signal Type" prompt="Select a Signal Type from the drop down list" sqref="I22:I33">
       <formula1>"Digital,PWM,0-10V,0-20mA"</formula1>
     </dataValidation>

</xml_diff>